<commit_message>
Lists with oData service, pagination and sorting
</commit_message>
<xml_diff>
--- a/MockupData.xlsx
+++ b/MockupData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Clubs" sheetId="2" r:id="rId1"/>
     <sheet name="Judoka" sheetId="4" r:id="rId2"/>
+    <sheet name="Competitions" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="530">
   <si>
     <t>Borås JK</t>
   </si>
@@ -1462,6 +1463,159 @@
   </si>
   <si>
     <t>ClubId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Haninge</t>
+  </si>
+  <si>
+    <t>Borlänge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Staffanstorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Borås</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Halmstad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stenungsund</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Skurup</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vilhelmina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lindesberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stockholm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Göteborg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sundsvall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lund</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Genarp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oxelösund</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karlstad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Helsingborg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kristianstad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Älvhögsborg</t>
+  </si>
+  <si>
+    <t>Skåneserien IV</t>
+  </si>
+  <si>
+    <t>SydCup IV och Veteran SM</t>
+  </si>
+  <si>
+    <t>-06 Adidas Challenge</t>
+  </si>
+  <si>
+    <t>National-Cup</t>
+  </si>
+  <si>
+    <t>GoCup II</t>
+  </si>
+  <si>
+    <t>Södra Judo Open III</t>
+  </si>
+  <si>
+    <t>Skåneserien 3</t>
+  </si>
+  <si>
+    <t>SydCup 3</t>
+  </si>
+  <si>
+    <t>Norra Norrlands DM</t>
+  </si>
+  <si>
+    <t>Linde Judo Open</t>
+  </si>
+  <si>
+    <t>Junior Swedish Open (J-Swop)</t>
+  </si>
+  <si>
+    <t>Borlänge Judo Open Resultat</t>
+  </si>
+  <si>
+    <t>Gothenburg Judo Open</t>
+  </si>
+  <si>
+    <t>Sundsvallscup</t>
+  </si>
+  <si>
+    <t>Budo-Nord Cup</t>
+  </si>
+  <si>
+    <t>Skåne-Serien II</t>
+  </si>
+  <si>
+    <t>-24 Trollträffen I</t>
+  </si>
+  <si>
+    <t>Senior SM 2016</t>
+  </si>
+  <si>
+    <t>Södra Judo Open 2</t>
+  </si>
+  <si>
+    <t>Sörmlandsträffen</t>
+  </si>
+  <si>
+    <t>Go Cup</t>
+  </si>
+  <si>
+    <t>Sun City Judo Open</t>
+  </si>
+  <si>
+    <t>Drakstadens Judo Cup</t>
+  </si>
+  <si>
+    <t>Adidas Challenge</t>
+  </si>
+  <si>
+    <t>Junior och Kadett SM</t>
+  </si>
+  <si>
+    <t>Helsingborg Judo Open</t>
+  </si>
+  <si>
+    <t>Södra Judo Open I</t>
+  </si>
+  <si>
+    <t>Skåneserien I</t>
+  </si>
+  <si>
+    <t>Kristianstad Judo Open Resultat</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>EventDate</t>
+  </si>
+  <si>
+    <t>Sql Command</t>
   </si>
 </sst>
 </file>
@@ -1507,15 +1661,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1524,6 +1682,53 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1572,53 +1777,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1633,12 +1791,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Clubs" displayName="Clubs" ref="A1:C41" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Clubs" displayName="Clubs" ref="A1:C41" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:C41"/>
   <tableColumns count="3">
     <tableColumn id="2" name="Name" dataDxfId="6"/>
-    <tableColumn id="4" name="Id" dataDxfId="3"/>
-    <tableColumn id="3" name="SqlCommand" dataDxfId="5"/>
+    <tableColumn id="4" name="Id" dataDxfId="5"/>
+    <tableColumn id="3" name="SqlCommand" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1655,14 +1813,29 @@
     <tableColumn id="2" name="FirstName"/>
     <tableColumn id="3" name="LastName"/>
     <tableColumn id="4" name="Birthyear"/>
-    <tableColumn id="5" name="ClubId" dataDxfId="2">
+    <tableColumn id="5" name="ClubId" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(Tabell5[[#This Row],[Club]],Clubs[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Personnumber" dataDxfId="1">
+    <tableColumn id="6" name="Personnumber" dataDxfId="2">
       <calculatedColumnFormula>TEXT(RANDBETWEEN(DATE(D2,1,1),DATE(D2,12,31)),"ååååmmdd") &amp; "-" &amp; RANDBETWEEN(1000,9999)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="SqlCommand" dataDxfId="0">
+    <tableColumn id="7" name="SqlCommand" dataDxfId="1">
       <calculatedColumnFormula>"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabell2" displayName="Tabell2" ref="A1:D30" totalsRowShown="0">
+  <autoFilter ref="A1:D30"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Location"/>
+    <tableColumn id="2" name="EventDate" dataDxfId="0"/>
+    <tableColumn id="3" name="Name"/>
+    <tableColumn id="4" name="Sql Command">
+      <calculatedColumnFormula>"insert into Competitions (Name, Location, EventDate) VALUES('"&amp;C2&amp;"', '"&amp;A2&amp;"','"&amp;TEXT(B2,"åååå-MM-dd")&amp;"');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2445,7 +2618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+    <sheetView topLeftCell="A219" workbookViewId="0">
       <selection activeCell="F248" sqref="F248"/>
     </sheetView>
   </sheetViews>
@@ -2502,11 +2675,11 @@
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F65" ca="1" si="0">TEXT(RANDBETWEEN(DATE(D2,1,1),DATE(D2,12,31)),"ååååmmdd") &amp; "-" &amp; RANDBETWEEN(1000,9999)</f>
-        <v>20030023-9109</v>
+        <v>20030011-2667</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gretha','ÖSTLIND','20030023-9109');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gretha','ÖSTLIND','20030011-2667');</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2528,11 +2701,11 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19860019-8749</v>
+        <v>19860003-1205</v>
       </c>
       <c r="G3" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES (' tim','ÖRN','19860019-8749');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES (' tim','ÖRN','19860003-1205');</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2554,11 +2727,11 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19710011-9379</v>
+        <v>19710013-4679</v>
       </c>
       <c r="G4" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Peter','ÅKESSON','19710011-9379');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Peter','ÅKESSON','19710013-4679');</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2580,11 +2753,11 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20050018-4000</v>
+        <v>20050029-5873</v>
       </c>
       <c r="G5" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','ÅBERG','20050018-4000');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','ÅBERG','20050029-5873');</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2606,11 +2779,11 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19940007-4778</v>
+        <v>19940023-4199</v>
       </c>
       <c r="G6" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Herolind','XHAFOLI','19940007-4778');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Herolind','XHAFOLI','19940023-4199');</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2632,11 +2805,11 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20030015-4302</v>
+        <v>20030027-9723</v>
       </c>
       <c r="G7" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','VIEBKE','20030015-4302');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','VIEBKE','20030027-9723');</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2658,11 +2831,11 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040014-1733</v>
+        <v>20040016-4276</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tuwa','WICKSTRÖM','20040014-1733');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tuwa','WICKSTRÖM','20040016-4276');</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2684,11 +2857,11 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020023-7137</v>
+        <v>20020029-2130</v>
       </c>
       <c r="G9" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hannes','WESSLÉN','20020023-7137');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hannes','WESSLÉN','20020029-2130');</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2710,11 +2883,11 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20030014-4578</v>
+        <v>20030009-3611</v>
       </c>
       <c r="G10" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Moa ','WENNSTAM','20030014-4578');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Moa ','WENNSTAM','20030009-3611');</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2736,11 +2909,11 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020017-6878</v>
+        <v>20020020-8562</v>
       </c>
       <c r="G11" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Känan','VELJE','20020017-6878');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Känan','VELJE','20020020-8562');</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2762,11 +2935,11 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19970020-1832</v>
+        <v>19970001-3006</v>
       </c>
       <c r="G12" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B12&amp;"','"&amp;C12&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pablo','VELAZCO','19970020-1832');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pablo','VELAZCO','19970001-3006');</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2788,11 +2961,11 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20050027-1144</v>
+        <v>20050007-8185</v>
       </c>
       <c r="G13" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B13&amp;"','"&amp;C13&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','WASSHOLM','20050027-1144');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','WASSHOLM','20050007-8185');</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,11 +2987,11 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20030027-8235</v>
+        <v>20030028-2366</v>
       </c>
       <c r="G14" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B14&amp;"','"&amp;C14&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Theodor','WASS','20030027-8235');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Theodor','WASS','20030028-2366');</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2840,11 +3013,11 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20010011-9478</v>
+        <v>20010019-3844</v>
       </c>
       <c r="G15" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B15&amp;"','"&amp;C15&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','ULMAN','20010011-9478');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','ULMAN','20010019-3844');</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2866,11 +3039,11 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040020-9988</v>
+        <v>20040018-6719</v>
       </c>
       <c r="G16" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amanda','TÖRNGREN','20040020-9988');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amanda','TÖRNGREN','20040018-6719');</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2892,11 +3065,11 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20000013-6266</v>
+        <v>20000010-6804</v>
       </c>
       <c r="G17" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B17&amp;"','"&amp;C17&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','TORKAR','20000013-6266');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','TORKAR','20000010-6804');</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2918,11 +3091,11 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020025-1185</v>
+        <v>20020012-7058</v>
       </c>
       <c r="G18" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B18&amp;"','"&amp;C18&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karl','THÖRSMAN','20020025-1185');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karl','THÖRSMAN','20020012-7058');</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2944,11 +3117,11 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040030-9837</v>
+        <v>20040007-5944</v>
       </c>
       <c r="G19" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B19&amp;"','"&amp;C19&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tea','THILFALK','20040030-9837');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tea','THILFALK','20040007-5944');</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2970,11 +3143,11 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19980017-2119</v>
+        <v>19980022-7572</v>
       </c>
       <c r="G20" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B20&amp;"','"&amp;C20&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Julia','TENGELIN','19980017-2119');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Julia','TENGELIN','19980022-7572');</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2996,11 +3169,11 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020027-9643</v>
+        <v>20020011-5060</v>
       </c>
       <c r="G21" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B21&amp;"','"&amp;C21&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pontus','SÖREM','20020027-9643');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pontus','SÖREM','20020011-5060');</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3022,11 +3195,11 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20050004-5299</v>
+        <v>20050029-3289</v>
       </c>
       <c r="G22" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B22&amp;"','"&amp;C22&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kalle','SVENBY','20050004-5299');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kalle','SVENBY','20050029-3289');</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3048,11 +3221,11 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040028-8744</v>
+        <v>20040004-5011</v>
       </c>
       <c r="G23" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B23&amp;"','"&amp;C23&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Stina','SVENBY','20040028-8744');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Stina','SVENBY','20040004-5011');</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -3074,11 +3247,11 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19990025-2606</v>
+        <v>19990016-8594</v>
       </c>
       <c r="G24" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B24&amp;"','"&amp;C24&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Noa','SWANLING','19990025-2606');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Noa','SWANLING','19990016-8594');</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3100,11 +3273,11 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20010020-7197</v>
+        <v>20010024-9689</v>
       </c>
       <c r="G25" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B25&amp;"','"&amp;C25&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Leon','SVALBERG','20010020-7197');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Leon','SVALBERG','20010024-9689');</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3126,11 +3299,11 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19860021-8215</v>
+        <v>19860015-9981</v>
       </c>
       <c r="G26" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B26&amp;"','"&amp;C26&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','SUNDQVIST','19860021-8215');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','SUNDQVIST','19860015-9981');</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3152,11 +3325,11 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20030001-8321</v>
+        <v>20030015-2372</v>
       </c>
       <c r="G27" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B27&amp;"','"&amp;C27&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Olivia','STRÖMBERG','20030001-8321');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Olivia','STRÖMBERG','20030015-2372');</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3178,11 +3351,11 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20010009-4764</v>
+        <v>20010020-8638</v>
       </c>
       <c r="G28" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B28&amp;"','"&amp;C28&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','STRANDBERG','20010009-4764');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','STRANDBERG','20010020-8638');</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3204,11 +3377,11 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20010027-5981</v>
+        <v>20010018-6228</v>
       </c>
       <c r="G29" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B29&amp;"','"&amp;C29&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','STINTZING','20010027-5981');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','STINTZING','20010018-6228');</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3230,11 +3403,11 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19990006-8307</v>
+        <v>19990017-4143</v>
       </c>
       <c r="G30" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B30&amp;"','"&amp;C30&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elin','STIGBORG','19990006-8307');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elin','STIGBORG','19990017-4143');</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3256,11 +3429,11 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19790029-1004</v>
+        <v>19790026-2576</v>
       </c>
       <c r="G31" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B31&amp;"','"&amp;C31&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Thomas','STENQVIST','19790029-1004');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Thomas','STENQVIST','19790026-2576');</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3282,11 +3455,11 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20000022-3170</v>
+        <v>20000025-8394</v>
       </c>
       <c r="G32" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B32&amp;"','"&amp;C32&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johanna','STENMAN','20000022-3170');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johanna','STENMAN','20000025-8394');</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3308,11 +3481,11 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20000013-1723</v>
+        <v>20000028-6353</v>
       </c>
       <c r="G33" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B33&amp;"','"&amp;C33&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hugo','STENERSEN','20000013-1723');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hugo','STENERSEN','20000028-6353');</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3334,11 +3507,11 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040012-8295</v>
+        <v>20040023-1851</v>
       </c>
       <c r="G34" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B34&amp;"','"&amp;C34&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ellen','STENBERG','20040012-8295');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ellen','STENBERG','20040023-1851');</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3360,11 +3533,11 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040018-4978</v>
+        <v>20040001-5580</v>
       </c>
       <c r="G35" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B35&amp;"','"&amp;C35&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hanna','STENBERG','20040018-4978');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hanna','STENBERG','20040001-5580');</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3386,11 +3559,11 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20000003-3348</v>
+        <v>20000030-4819</v>
       </c>
       <c r="G36" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B36&amp;"','"&amp;C36&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linn','STENBERG','20000003-3348');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linn','STENBERG','20000030-4819');</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3412,11 +3585,11 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040026-7614</v>
+        <v>20040003-5836</v>
       </c>
       <c r="G37" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B37&amp;"','"&amp;C37&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Axel','STEN','20040026-7614');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Axel','STEN','20040003-5836');</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3438,11 +3611,11 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20030005-7273</v>
+        <v>20030003-6932</v>
       </c>
       <c r="G38" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B38&amp;"','"&amp;C38&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Wilhelm','STEINBECK','20030005-7273');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Wilhelm','STEINBECK','20030003-6932');</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3464,11 +3637,11 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20050020-2625</v>
+        <v>20050013-4067</v>
       </c>
       <c r="G39" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B39&amp;"','"&amp;C39&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Oliver','STANGDELL','20050020-2625');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Oliver','STANGDELL','20050013-4067');</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3490,11 +3663,11 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20040029-2889</v>
+        <v>20040015-9219</v>
       </c>
       <c r="G40" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B40&amp;"','"&amp;C40&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alvin','STALLGÅRD','20040029-2889');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alvin','STALLGÅRD','20040015-9219');</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3516,11 +3689,11 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19990004-9768</v>
+        <v>19990012-9743</v>
       </c>
       <c r="G41" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B41&amp;"','"&amp;C41&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Fanny','SPÅNGBERG','19990004-9768');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Fanny','SPÅNGBERG','19990012-9743');</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3542,11 +3715,11 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020001-6574</v>
+        <v>20020017-5053</v>
       </c>
       <c r="G42" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B42&amp;"','"&amp;C42&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Andre','SOLOMI','20020001-6574');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Andre','SOLOMI','20020017-5053');</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3568,11 +3741,11 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19880004-8381</v>
+        <v>19880006-5619</v>
       </c>
       <c r="G43" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B43&amp;"','"&amp;C43&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Vytautas','SKILINSKAS','19880004-8381');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Vytautas','SKILINSKAS','19880006-5619');</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3594,11 +3767,11 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20010028-2597</v>
+        <v>20010009-9227</v>
       </c>
       <c r="G44" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B44&amp;"','"&amp;C44&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','SJÖSTEDT','20010028-2597');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','SJÖSTEDT','20010009-9227');</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3620,11 +3793,11 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20010006-8898</v>
+        <v>20010004-3657</v>
       </c>
       <c r="G45" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B45&amp;"','"&amp;C45&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonathan','SJÖGREN','20010006-8898');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonathan','SJÖGREN','20010004-3657');</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3646,11 +3819,11 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020023-9289</v>
+        <v>20020001-7781</v>
       </c>
       <c r="G46" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B46&amp;"','"&amp;C46&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nicholas','SJÖGREN','20020023-9289');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nicholas','SJÖGREN','20020001-7781');</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3672,11 +3845,11 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19990023-1285</v>
+        <v>19990010-5041</v>
       </c>
       <c r="G47" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B47&amp;"','"&amp;C47&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','SIKSTRÖM','19990023-1285');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','SIKSTRÖM','19990010-5041');</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3698,11 +3871,11 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19940010-8467</v>
+        <v>19940017-7390</v>
       </c>
       <c r="G48" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B48&amp;"','"&amp;C48&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sahand','SHOKOHI','19940010-8467');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sahand','SHOKOHI','19940017-7390');</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3724,11 +3897,11 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020030-8036</v>
+        <v>20020003-2085</v>
       </c>
       <c r="G49" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B49&amp;"','"&amp;C49&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonay','SANTANA','20020030-8036');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonay','SANTANA','20020003-2085');</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3750,11 +3923,11 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020004-3751</v>
+        <v>20020017-8374</v>
       </c>
       <c r="G50" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B50&amp;"','"&amp;C50&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rebecca','SANDBERG','20020004-3751');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rebecca','SANDBERG','20020017-8374');</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3776,11 +3949,11 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19970023-1219</v>
+        <v>19970002-6549</v>
       </c>
       <c r="G51" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B51&amp;"','"&amp;C51&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Eric','RÖSSEL','19970023-1219');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Eric','RÖSSEL','19970002-6549');</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3802,11 +3975,11 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20030026-6709</v>
+        <v>20030008-1215</v>
       </c>
       <c r="G52" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B52&amp;"','"&amp;C52&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Wilma','RÖSSEL','20030026-6709');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Wilma','RÖSSEL','20030008-1215');</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3828,11 +4001,11 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20050023-7455</v>
+        <v>20050027-1922</v>
       </c>
       <c r="G53" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B53&amp;"','"&amp;C53&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nikolaj','RUPI','20050023-7455');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nikolaj','RUPI','20050027-1922');</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3854,11 +4027,11 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20030031-7082</v>
+        <v>20030010-1692</v>
       </c>
       <c r="G54" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B54&amp;"','"&amp;C54&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Lukas','ROSWALL','20030031-7082');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Lukas','ROSWALL','20030010-1692');</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3880,11 +4053,11 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20000028-7713</v>
+        <v>20000006-9412</v>
       </c>
       <c r="G55" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B55&amp;"','"&amp;C55&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mitchell','ROMERO','20000028-7713');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mitchell','ROMERO','20000006-9412');</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3906,11 +4079,11 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020031-7621</v>
+        <v>20020022-3858</v>
       </c>
       <c r="G56" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B56&amp;"','"&amp;C56&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','RODELL','20020031-7621');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','RODELL','20020022-3858');</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3932,11 +4105,11 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19990013-7910</v>
+        <v>19990001-7561</v>
       </c>
       <c r="G57" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B57&amp;"','"&amp;C57&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','RITTFELDT','19990013-7910');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','RITTFELDT','19990001-7561');</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3958,11 +4131,11 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19960005-4379</v>
+        <v>19960012-7148</v>
       </c>
       <c r="G58" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B58&amp;"','"&amp;C58&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Edvin','RINDE','19960005-4379');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Edvin','RINDE','19960012-7148');</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3984,11 +4157,11 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20000025-6476</v>
+        <v>20000006-8960</v>
       </c>
       <c r="G59" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B59&amp;"','"&amp;C59&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nikita','RIETZ','20000025-6476');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nikita','RIETZ','20000006-8960');</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -4010,11 +4183,11 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020029-6299</v>
+        <v>20020030-6346</v>
       </c>
       <c r="G60" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B60&amp;"','"&amp;C60&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','RIDELL','20020029-6299');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','RIDELL','20020030-6346');</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -4036,11 +4209,11 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19970006-2939</v>
+        <v>19970009-6903</v>
       </c>
       <c r="G61" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B61&amp;"','"&amp;C61&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Adam','RENKIELSKI','19970006-2939');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Adam','RENKIELSKI','19970009-6903');</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -4062,11 +4235,11 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19990028-2480</v>
+        <v>19990027-4542</v>
       </c>
       <c r="G62" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B62&amp;"','"&amp;C62&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Shawn','REDDY','19990028-2480');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Shawn','REDDY','19990027-4542');</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -4088,11 +4261,11 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20020013-6519</v>
+        <v>20020015-2162</v>
       </c>
       <c r="G63" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B63&amp;"','"&amp;C63&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Leo','RAND','20020013-6519');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Leo','RAND','20020015-2162');</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -4114,11 +4287,11 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20000022-6802</v>
+        <v>20000006-2807</v>
       </c>
       <c r="G64" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B64&amp;"','"&amp;C64&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Felicia','PÅLSSON','20000022-6802');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Felicia','PÅLSSON','20000006-2807');</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -4140,11 +4313,11 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19990024-8539</v>
+        <v>19990001-9309</v>
       </c>
       <c r="G65" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B65&amp;"','"&amp;C65&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mathilde','PILEMANN','19990024-8539');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mathilde','PILEMANN','19990001-9309');</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -4166,11 +4339,11 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" ref="F66:F129" ca="1" si="1">TEXT(RANDBETWEEN(DATE(D66,1,1),DATE(D66,12,31)),"ååååmmdd") &amp; "-" &amp; RANDBETWEEN(1000,9999)</f>
-        <v>20020017-8492</v>
+        <v>20020018-7034</v>
       </c>
       <c r="G66" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B66&amp;"','"&amp;C66&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Albin','PERSSON','20020017-8492');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Albin','PERSSON','20020018-7034');</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -4192,11 +4365,11 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20040002-5497</v>
+        <v>20040031-7677</v>
       </c>
       <c r="G67" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B67&amp;"','"&amp;C67&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Malte','PERSSON','20040002-5497');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Malte','PERSSON','20040031-7677');</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -4218,11 +4391,11 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020008-3690</v>
+        <v>20020006-7986</v>
       </c>
       <c r="G68" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B68&amp;"','"&amp;C68&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Heydar','PASHAEV','20020008-3690');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Heydar','PASHAEV','20020006-7986');</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -4244,11 +4417,11 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20010004-9039</v>
+        <v>20010007-4059</v>
       </c>
       <c r="G69" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B69&amp;"','"&amp;C69&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pasha','PASHAEV','20010004-9039');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pasha','PASHAEV','20010007-4059');</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -4270,11 +4443,11 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20040005-8043</v>
+        <v>20040018-3617</v>
       </c>
       <c r="G70" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B70&amp;"','"&amp;C70&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jacob','PALMQVIST','20040005-8043');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jacob','PALMQVIST','20040018-3617');</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -4296,11 +4469,11 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20010005-2963</v>
+        <v>20010004-1910</v>
       </c>
       <c r="G71" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B71&amp;"','"&amp;C71&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Axel','OSCARSSON','20010005-2963');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Axel','OSCARSSON','20010004-1910');</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4322,11 +4495,11 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19970031-8576</v>
+        <v>19970029-3261</v>
       </c>
       <c r="G72" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B72&amp;"','"&amp;C72&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Samuel','ÒMARSSON','19970031-8576');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Samuel','ÒMARSSON','19970029-3261');</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -4348,11 +4521,11 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19970013-6211</v>
+        <v>19970016-6622</v>
       </c>
       <c r="G73" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B73&amp;"','"&amp;C73&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','OLSSON','19970013-6211');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','OLSSON','19970016-6622');</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -4374,11 +4547,11 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20030013-5608</v>
+        <v>20030029-8155</v>
       </c>
       <c r="G74" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B74&amp;"','"&amp;C74&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','OLOFSSON','20030013-5608');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','OLOFSSON','20030029-8155');</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -4400,11 +4573,11 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20010012-2269</v>
+        <v>20010028-4594</v>
       </c>
       <c r="G75" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B75&amp;"','"&amp;C75&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sebastian','OLOFSSON','20010012-2269');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sebastian','OLOFSSON','20010028-4594');</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4426,11 +4599,11 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020001-2703</v>
+        <v>20020014-4810</v>
       </c>
       <c r="G76" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B76&amp;"','"&amp;C76&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','NYMAN','20020001-2703');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','NYMAN','20020014-4810');</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4452,11 +4625,11 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19990017-3030</v>
+        <v>19990026-4988</v>
       </c>
       <c r="G77" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B77&amp;"','"&amp;C77&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tim','NYLANDER','19990017-3030');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tim','NYLANDER','19990026-4988');</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4478,11 +4651,11 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20030011-2483</v>
+        <v>20030026-2381</v>
       </c>
       <c r="G78" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B78&amp;"','"&amp;C78&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nora','NYBY','20030011-2483');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Nora','NYBY','20030026-2381');</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4504,11 +4677,11 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19980029-3082</v>
+        <v>19980010-3963</v>
       </c>
       <c r="G79" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B79&amp;"','"&amp;C79&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','NORMAN','19980029-3082');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','NORMAN','19980010-3963');</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4530,11 +4703,11 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19990008-1719</v>
+        <v>19990004-8138</v>
       </c>
       <c r="G80" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B80&amp;"','"&amp;C80&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Richard bergwall','NILSSON','19990008-1719');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Richard bergwall','NILSSON','19990004-8138');</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4556,11 +4729,11 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20000012-5312</v>
+        <v>20000019-5218</v>
       </c>
       <c r="G81" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B81&amp;"','"&amp;C81&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Erik','NICODEMI','20000012-5312');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Erik','NICODEMI','20000019-5218');</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4582,11 +4755,11 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20030001-9773</v>
+        <v>20030016-9002</v>
       </c>
       <c r="G82" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B82&amp;"','"&amp;C82&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karim','NABI','20030001-9773');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karim','NABI','20030016-9002');</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4608,11 +4781,11 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20030011-4843</v>
+        <v>20030007-2276</v>
       </c>
       <c r="G83" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B83&amp;"','"&amp;C83&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','MÅRTENSSON','20030011-4843');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','MÅRTENSSON','20030007-2276');</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4634,11 +4807,11 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20050013-5482</v>
+        <v>20050001-8608</v>
       </c>
       <c r="G84" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B84&amp;"','"&amp;C84&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linnea','MÅRTENSSON','20050013-5482');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linnea','MÅRTENSSON','20050001-8608');</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4660,11 +4833,11 @@
       </c>
       <c r="F85" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19960014-5079</v>
+        <v>19960024-8653</v>
       </c>
       <c r="G85" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B85&amp;"','"&amp;C85&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Behar','MUSLIJA','19960014-5079');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Behar','MUSLIJA','19960024-8653');</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4686,11 +4859,11 @@
       </c>
       <c r="F86" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19960012-8305</v>
+        <v>19960022-5310</v>
       </c>
       <c r="G86" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B86&amp;"','"&amp;C86&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Abdullah','MUSA','19960012-8305');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Abdullah','MUSA','19960022-5310');</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4712,11 +4885,11 @@
       </c>
       <c r="F87" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19990014-9681</v>
+        <v>19990026-6951</v>
       </c>
       <c r="G87" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B87&amp;"','"&amp;C87&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karin','MOREAU','19990014-9681');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karin','MOREAU','19990026-6951');</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4738,11 +4911,11 @@
       </c>
       <c r="F88" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19950007-3925</v>
+        <v>19950001-6986</v>
       </c>
       <c r="G88" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B88&amp;"','"&amp;C88&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sajad','MOHAMMED ALI','19950007-3925');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sajad','MOHAMMED ALI','19950001-6986');</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4764,11 +4937,11 @@
       </c>
       <c r="F89" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20040020-2626</v>
+        <v>20040027-3788</v>
       </c>
       <c r="G89" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B89&amp;"','"&amp;C89&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Maxim','MOCANOSKI','20040020-2626');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Maxim','MOCANOSKI','20040027-3788');</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4790,11 +4963,11 @@
       </c>
       <c r="F90" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20040004-7661</v>
+        <v>20040011-7034</v>
       </c>
       <c r="G90" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B90&amp;"','"&amp;C90&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Lukas','MITROVIC','20040004-7661');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Lukas','MITROVIC','20040011-7034');</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4816,11 +4989,11 @@
       </c>
       <c r="F91" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20040019-6281</v>
+        <v>20040003-8461</v>
       </c>
       <c r="G91" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B91&amp;"','"&amp;C91&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elin','MILLESSON','20040019-6281');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elin','MILLESSON','20040003-8461');</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4842,11 +5015,11 @@
       </c>
       <c r="F92" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020023-5560</v>
+        <v>20020009-8614</v>
       </c>
       <c r="G92" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B92&amp;"','"&amp;C92&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Esben','METZSCH','20020023-5560');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Esben','METZSCH','20020009-8614');</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4868,11 +5041,11 @@
       </c>
       <c r="F93" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020027-9067</v>
+        <v>20020010-5035</v>
       </c>
       <c r="G93" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B93&amp;"','"&amp;C93&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Viktor','MENSHIKOV','20020027-9067');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Viktor','MENSHIKOV','20020010-5035');</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4894,11 +5067,11 @@
       </c>
       <c r="F94" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20000028-3925</v>
+        <v>20000015-6285</v>
       </c>
       <c r="G94" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B94&amp;"','"&amp;C94&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Robert','MEMETI','20000028-3925');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Robert','MEMETI','20000015-6285');</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4920,11 +5093,11 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19970030-5136</v>
+        <v>19970009-9669</v>
       </c>
       <c r="G95" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B95&amp;"','"&amp;C95&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Klara','MATTSSON','19970030-5136');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Klara','MATTSSON','19970009-9669');</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4946,11 +5119,11 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20030024-9515</v>
+        <v>20030028-7965</v>
       </c>
       <c r="G96" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B96&amp;"','"&amp;C96&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pelle','MATTSSON','20030024-9515');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pelle','MATTSSON','20030028-7965');</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4972,11 +5145,11 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20050026-7177</v>
+        <v>20050015-5947</v>
       </c>
       <c r="G97" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B97&amp;"','"&amp;C97&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ville','MATTSSON','20050026-7177');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ville','MATTSSON','20050015-5947');</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4998,11 +5171,11 @@
       </c>
       <c r="F98" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19870009-7843</v>
+        <v>19870006-7639</v>
       </c>
       <c r="G98" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B98&amp;"','"&amp;C98&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sider','MARTINOV','19870009-7843');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sider','MARTINOV','19870006-7639');</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -5024,11 +5197,11 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19970016-5218</v>
+        <v>19970003-6841</v>
       </c>
       <c r="G99" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B99&amp;"','"&amp;C99&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Masiollah','MAQSOUDI','19970016-5218');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Masiollah','MAQSOUDI','19970003-6841');</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -5050,11 +5223,11 @@
       </c>
       <c r="F100" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020023-4423</v>
+        <v>20020029-7678</v>
       </c>
       <c r="G100" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B100&amp;"','"&amp;C100&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Simon','MALMROS','20020023-4423');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Simon','MALMROS','20020029-7678');</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -5076,11 +5249,11 @@
       </c>
       <c r="F101" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19990031-6696</v>
+        <v>19990008-6463</v>
       </c>
       <c r="G101" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B101&amp;"','"&amp;C101&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Theodor','MALMQVIST','19990031-6696');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Theodor','MALMQVIST','19990008-6463');</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -5102,11 +5275,11 @@
       </c>
       <c r="F102" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20040008-3078</v>
+        <v>20040017-7883</v>
       </c>
       <c r="G102" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B102&amp;"','"&amp;C102&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pascal','MALMQUIST','20040008-3078');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pascal','MALMQUIST','20040017-7883');</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -5128,11 +5301,11 @@
       </c>
       <c r="F103" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19990020-6254</v>
+        <v>19990015-2935</v>
       </c>
       <c r="G103" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B103&amp;"','"&amp;C103&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ismail','MALKOC','19990020-6254');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ismail','MALKOC','19990015-2935');</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -5154,11 +5327,11 @@
       </c>
       <c r="F104" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020001-9619</v>
+        <v>20020011-7104</v>
       </c>
       <c r="G104" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B104&amp;"','"&amp;C104&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('César','MAGNUSSON','20020001-9619');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('César','MAGNUSSON','20020011-7104');</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -5180,11 +5353,11 @@
       </c>
       <c r="F105" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19970002-5306</v>
+        <v>19970004-8032</v>
       </c>
       <c r="G105" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B105&amp;"','"&amp;C105&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','MAATOUG','19970002-5306');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','MAATOUG','19970004-8032');</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -5206,11 +5379,11 @@
       </c>
       <c r="F106" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20050024-1428</v>
+        <v>20050026-4276</v>
       </c>
       <c r="G106" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B106&amp;"','"&amp;C106&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl viggo','LÖVENSTIERNE','20050024-1428');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl viggo','LÖVENSTIERNE','20050026-4276');</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -5232,11 +5405,11 @@
       </c>
       <c r="F107" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020005-2730</v>
+        <v>20020004-7241</v>
       </c>
       <c r="G107" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B107&amp;"','"&amp;C107&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Beatrice','LUNDIN','20020005-2730');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Beatrice','LUNDIN','20020004-7241');</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -5258,11 +5431,11 @@
       </c>
       <c r="F108" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20000004-2131</v>
+        <v>20000002-4620</v>
       </c>
       <c r="G108" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B108&amp;"','"&amp;C108&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Albin','LUNDHOLM','20000004-2131');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Albin','LUNDHOLM','20000002-4620');</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -5284,11 +5457,11 @@
       </c>
       <c r="F109" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19940018-5572</v>
+        <v>19940015-9796</v>
       </c>
       <c r="G109" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B109&amp;"','"&amp;C109&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('David','LUNDGREN','19940018-5572');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('David','LUNDGREN','19940015-9796');</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -5310,11 +5483,11 @@
       </c>
       <c r="F110" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20040026-8602</v>
+        <v>20040015-6721</v>
       </c>
       <c r="G110" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B110&amp;"','"&amp;C110&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Milla','LUNDBLADH','20040026-8602');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Milla','LUNDBLADH','20040015-6721');</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -5336,11 +5509,11 @@
       </c>
       <c r="F111" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020012-9696</v>
+        <v>20020031-7314</v>
       </c>
       <c r="G111" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B111&amp;"','"&amp;C111&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl ','LJUNGQVIST','20020012-9696');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl ','LJUNGQVIST','20020031-7314');</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -5362,11 +5535,11 @@
       </c>
       <c r="F112" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20010028-5367</v>
+        <v>20010005-2582</v>
       </c>
       <c r="G112" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B112&amp;"','"&amp;C112&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Konrad ','LJUNGQVIST','20010028-5367');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Konrad ','LJUNGQVIST','20010005-2582');</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -5388,11 +5561,11 @@
       </c>
       <c r="F113" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20030013-5949</v>
+        <v>20030017-3272</v>
       </c>
       <c r="G113" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B113&amp;"','"&amp;C113&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Melker ','LJUNGQVIST','20030013-5949');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Melker ','LJUNGQVIST','20030017-3272');</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -5414,11 +5587,11 @@
       </c>
       <c r="F114" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20010025-6357</v>
+        <v>20010015-7282</v>
       </c>
       <c r="G114" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B114&amp;"','"&amp;C114&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Michelle','LJUNG','20010025-6357');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Michelle','LJUNG','20010015-7282');</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -5440,11 +5613,11 @@
       </c>
       <c r="F115" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20030021-8623</v>
+        <v>20030027-4473</v>
       </c>
       <c r="G115" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B115&amp;"','"&amp;C115&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonatan','LINGMERTH','20030021-8623');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonatan','LINGMERTH','20030027-4473');</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -5466,11 +5639,11 @@
       </c>
       <c r="F116" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020008-1773</v>
+        <v>20020018-1849</v>
       </c>
       <c r="G116" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B116&amp;"','"&amp;C116&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','LINDGREN','20020008-1773');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','LINDGREN','20020018-1849');</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -5492,11 +5665,11 @@
       </c>
       <c r="F117" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19880010-6438</v>
+        <v>19880005-2417</v>
       </c>
       <c r="G117" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B117&amp;"','"&amp;C117&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johannes','LINDGREN','19880010-6438');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johannes','LINDGREN','19880005-2417');</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -5518,11 +5691,11 @@
       </c>
       <c r="F118" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19910023-6960</v>
+        <v>19910007-6255</v>
       </c>
       <c r="G118" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B118&amp;"','"&amp;C118&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ulf','LINDBLOM','19910023-6960');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ulf','LINDBLOM','19910007-6255');</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -5544,11 +5717,11 @@
       </c>
       <c r="F119" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20050004-5473</v>
+        <v>20050003-5439</v>
       </c>
       <c r="G119" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B119&amp;"','"&amp;C119&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexandra','LIGNELL','20050004-5473');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexandra','LIGNELL','20050003-5439');</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -5570,11 +5743,11 @@
       </c>
       <c r="F120" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20050016-1720</v>
+        <v>20050015-3903</v>
       </c>
       <c r="G120" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B120&amp;"','"&amp;C120&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','LIGNELL','20050016-1720');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','LIGNELL','20050015-3903');</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -5596,11 +5769,11 @@
       </c>
       <c r="F121" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020003-3595</v>
+        <v>20020014-4108</v>
       </c>
       <c r="G121" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B121&amp;"','"&amp;C121&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('David','LEVY','20020003-3595');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('David','LEVY','20020014-4108');</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -5622,11 +5795,11 @@
       </c>
       <c r="F122" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20000024-7286</v>
+        <v>20000002-9501</v>
       </c>
       <c r="G122" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B122&amp;"','"&amp;C122&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tilda','LENNARTSSON','20000024-7286');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tilda','LENNARTSSON','20000002-9501');</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -5648,11 +5821,11 @@
       </c>
       <c r="F123" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19960001-4948</v>
+        <v>19960022-5196</v>
       </c>
       <c r="G123" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B123&amp;"','"&amp;C123&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Daniel','LEGRAF','19960001-4948');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Daniel','LEGRAF','19960022-5196');</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -5674,11 +5847,11 @@
       </c>
       <c r="F124" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19870014-1289</v>
+        <v>19870013-7175</v>
       </c>
       <c r="G124" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B124&amp;"','"&amp;C124&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sonata','LATISEVICIUTE','19870014-1289');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sonata','LATISEVICIUTE','19870013-7175');</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -5700,11 +5873,11 @@
       </c>
       <c r="F125" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020025-5863</v>
+        <v>20020019-7589</v>
       </c>
       <c r="G125" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B125&amp;"','"&amp;C125&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Aleksander','LARSSON','20020025-5863');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Aleksander','LARSSON','20020019-7589');</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -5726,11 +5899,11 @@
       </c>
       <c r="F126" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19920026-9830</v>
+        <v>19920024-4838</v>
       </c>
       <c r="G126" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B126&amp;"','"&amp;C126&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Edvin','LARSSON','19920026-9830');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Edvin','LARSSON','19920024-4838');</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -5752,11 +5925,11 @@
       </c>
       <c r="F127" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20050007-8145</v>
+        <v>20050031-1647</v>
       </c>
       <c r="G127" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B127&amp;"','"&amp;C127&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Engla','LARSSON','20050007-8145');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Engla','LARSSON','20050031-1647');</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -5778,11 +5951,11 @@
       </c>
       <c r="F128" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20050017-2905</v>
+        <v>20050022-2050</v>
       </c>
       <c r="G128" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B128&amp;"','"&amp;C128&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Erik','LARSSON','20050017-2905');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Erik','LARSSON','20050022-2050');</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -5804,11 +5977,11 @@
       </c>
       <c r="F129" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>20020006-2757</v>
+        <v>20020024-3911</v>
       </c>
       <c r="G129" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B129&amp;"','"&amp;C129&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Miljohn','LARSSON','20020006-2757');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Miljohn','LARSSON','20020024-3911');</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -5830,11 +6003,11 @@
       </c>
       <c r="F130" t="str">
         <f t="shared" ref="F130:F193" ca="1" si="2">TEXT(RANDBETWEEN(DATE(D130,1,1),DATE(D130,12,31)),"ååååmmdd") &amp; "-" &amp; RANDBETWEEN(1000,9999)</f>
-        <v>20040001-3916</v>
+        <v>20040028-9598</v>
       </c>
       <c r="G130" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B130&amp;"','"&amp;C130&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Smilla','LARSSON','20040001-3916');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Smilla','LARSSON','20040028-9598');</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -5856,11 +6029,11 @@
       </c>
       <c r="F131" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020017-9538</v>
+        <v>20020021-6225</v>
       </c>
       <c r="G131" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B131&amp;"','"&amp;C131&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Thim','LARSSON','20020017-9538');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Thim','LARSSON','20020021-6225');</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -5882,11 +6055,11 @@
       </c>
       <c r="F132" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030030-5614</v>
+        <v>20030002-3009</v>
       </c>
       <c r="G132" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B132&amp;"','"&amp;C132&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','LARSSON','20030030-5614');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','LARSSON','20030002-3009');</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -5908,11 +6081,11 @@
       </c>
       <c r="F133" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030008-5601</v>
+        <v>20030019-4263</v>
       </c>
       <c r="G133" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B133&amp;"','"&amp;C133&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonatha','LANDGREN','20030008-5601');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonatha','LANDGREN','20030019-4263');</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -5934,11 +6107,11 @@
       </c>
       <c r="F134" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19980030-2959</v>
+        <v>19980021-2258</v>
       </c>
       <c r="G134" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B134&amp;"','"&amp;C134&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rebecca','LANDEN','19980030-2959');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rebecca','LANDEN','19980021-2258');</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -5960,11 +6133,11 @@
       </c>
       <c r="F135" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010016-1106</v>
+        <v>20010016-6647</v>
       </c>
       <c r="G135" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B135&amp;"','"&amp;C135&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','KÄLLBERG','20010016-1106');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','KÄLLBERG','20010016-6647');</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -5986,11 +6159,11 @@
       </c>
       <c r="F136" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19990028-6240</v>
+        <v>19990026-1614</v>
       </c>
       <c r="G136" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B136&amp;"','"&amp;C136&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sandra','KÄLLBERG','19990028-6240');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sandra','KÄLLBERG','19990026-1614');</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -6012,11 +6185,11 @@
       </c>
       <c r="F137" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010024-5140</v>
+        <v>20010026-1937</v>
       </c>
       <c r="G137" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B137&amp;"','"&amp;C137&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','KROCKSTÄDE','20010024-5140');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','KROCKSTÄDE','20010026-1937');</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -6038,11 +6211,11 @@
       </c>
       <c r="F138" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020021-8748</v>
+        <v>20020008-7707</v>
       </c>
       <c r="G138" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B138&amp;"','"&amp;C138&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','KJELLDAHL','20020021-8748');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kevin','KJELLDAHL','20020008-7707');</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -6064,11 +6237,11 @@
       </c>
       <c r="F139" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19990019-4445</v>
+        <v>19990018-3453</v>
       </c>
       <c r="G139" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B139&amp;"','"&amp;C139&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Adrian','KIWATKOWSKI','19990019-4445');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Adrian','KIWATKOWSKI','19990018-3453');</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -6090,11 +6263,11 @@
       </c>
       <c r="F140" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010027-1365</v>
+        <v>20010025-7820</v>
       </c>
       <c r="G140" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B140&amp;"','"&amp;C140&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hannes','KIHLSTRÖM','20010027-1365');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hannes','KIHLSTRÖM','20010025-7820');</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -6116,11 +6289,11 @@
       </c>
       <c r="F141" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19970010-2581</v>
+        <v>19970016-5476</v>
       </c>
       <c r="G141" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B141&amp;"','"&amp;C141&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Dogana amin','KHALOUF','19970010-2581');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Dogana amin','KHALOUF','19970016-5476');</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -6142,11 +6315,11 @@
       </c>
       <c r="F142" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010027-5400</v>
+        <v>20010028-9912</v>
       </c>
       <c r="G142" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B142&amp;"','"&amp;C142&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Susanna','KAZEMIFAR','20010027-5400');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Susanna','KAZEMIFAR','20010028-9912');</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -6168,11 +6341,11 @@
       </c>
       <c r="F143" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010017-3166</v>
+        <v>20010013-7651</v>
       </c>
       <c r="G143" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B143&amp;"','"&amp;C143&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emma','KAUPPINEN','20010017-3166');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emma','KAUPPINEN','20010013-7651');</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -6194,11 +6367,11 @@
       </c>
       <c r="F144" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19980013-1644</v>
+        <v>19980030-6758</v>
       </c>
       <c r="G144" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B144&amp;"','"&amp;C144&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Samuel','KAUPPINEN','19980013-1644');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Samuel','KAUPPINEN','19980030-6758');</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -6220,11 +6393,11 @@
       </c>
       <c r="F145" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20000025-4046</v>
+        <v>20000029-8019</v>
       </c>
       <c r="G145" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B145&amp;"','"&amp;C145&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','KARLSSON','20000025-4046');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','KARLSSON','20000029-8019');</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -6246,11 +6419,11 @@
       </c>
       <c r="F146" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19980003-9192</v>
+        <v>19980022-3824</v>
       </c>
       <c r="G146" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B146&amp;"','"&amp;C146&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Vincent','KARAGIANNIS','19980003-9192');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Vincent','KARAGIANNIS','19980022-3824');</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -6272,11 +6445,11 @@
       </c>
       <c r="F147" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20050029-6799</v>
+        <v>20050005-6487</v>
       </c>
       <c r="G147" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B147&amp;"','"&amp;C147&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mateo','JÖNSSON WALDES','20050029-6799');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mateo','JÖNSSON WALDES','20050005-6487');</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -6298,11 +6471,11 @@
       </c>
       <c r="F148" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030006-3255</v>
+        <v>20030002-5764</v>
       </c>
       <c r="G148" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B148&amp;"','"&amp;C148&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustav','JÖNSSON','20030006-3255');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustav','JÖNSSON','20030002-5764');</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -6324,11 +6497,11 @@
       </c>
       <c r="F149" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20050003-6203</v>
+        <v>20050015-7849</v>
       </c>
       <c r="G149" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B149&amp;"','"&amp;C149&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jenny','JÖNSSON','20050003-6203');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jenny','JÖNSSON','20050015-7849');</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -6350,11 +6523,11 @@
       </c>
       <c r="F150" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030017-7036</v>
+        <v>20030013-1323</v>
       </c>
       <c r="G150" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B150&amp;"','"&amp;C150&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linus','JÖNSSON','20030017-7036');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linus','JÖNSSON','20030013-1323');</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -6376,11 +6549,11 @@
       </c>
       <c r="F151" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010020-6476</v>
+        <v>20010014-5968</v>
       </c>
       <c r="G151" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B151&amp;"','"&amp;C151&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Daniel','JÄRPE','20010020-6476');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Daniel','JÄRPE','20010014-5968');</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -6402,11 +6575,11 @@
       </c>
       <c r="F152" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20000020-2013</v>
+        <v>20000009-9561</v>
       </c>
       <c r="G152" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B152&amp;"','"&amp;C152&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Oscar','JONASSON','20000020-2013');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Oscar','JONASSON','20000009-9561');</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -6428,11 +6601,11 @@
       </c>
       <c r="F153" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020016-6266</v>
+        <v>20020007-4714</v>
       </c>
       <c r="G153" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B153&amp;"','"&amp;C153&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amy','JOHNSSON','20020016-6266');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amy','JOHNSSON','20020007-4714');</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -6454,11 +6627,11 @@
       </c>
       <c r="F154" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020011-6213</v>
+        <v>20020023-4601</v>
       </c>
       <c r="G154" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B154&amp;"','"&amp;C154&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl','JOHANSSON','20020011-6213');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl','JOHANSSON','20020023-4601');</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -6480,11 +6653,11 @@
       </c>
       <c r="F155" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19990015-7186</v>
+        <v>19990006-6942</v>
       </c>
       <c r="G155" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B155&amp;"','"&amp;C155&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carolina','JOHANSSON','19990015-7186');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carolina','JOHANSSON','19990006-6942');</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -6506,11 +6679,11 @@
       </c>
       <c r="F156" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19980020-4108</v>
+        <v>19980019-2216</v>
       </c>
       <c r="G156" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B156&amp;"','"&amp;C156&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Dan','JOHANSSON','19980020-4108');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Dan','JOHANSSON','19980019-2216');</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -6532,11 +6705,11 @@
       </c>
       <c r="F157" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19950027-2498</v>
+        <v>19950017-2313</v>
       </c>
       <c r="G157" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B157&amp;"','"&amp;C157&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Fredrik','JOHANSSON','19950027-2498');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Fredrik','JOHANSSON','19950017-2313');</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -6558,11 +6731,11 @@
       </c>
       <c r="F158" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010006-7447</v>
+        <v>20010027-2043</v>
       </c>
       <c r="G158" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B158&amp;"','"&amp;C158&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hanna','JOHANSSON','20010006-7447');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hanna','JOHANSSON','20010027-2043');</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -6584,11 +6757,11 @@
       </c>
       <c r="F159" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20040004-3868</v>
+        <v>20040003-8399</v>
       </c>
       <c r="G159" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B159&amp;"','"&amp;C159&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('John','JOHANSSON','20040004-3868');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('John','JOHANSSON','20040003-8399');</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -6610,11 +6783,11 @@
       </c>
       <c r="F160" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19980007-1356</v>
+        <v>19980001-5623</v>
       </c>
       <c r="G160" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B160&amp;"','"&amp;C160&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mattias','JOHANSSON','19980007-1356');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mattias','JOHANSSON','19980001-5623');</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -6636,11 +6809,11 @@
       </c>
       <c r="F161" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020009-6529</v>
+        <v>20020018-3912</v>
       </c>
       <c r="G161" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B161&amp;"','"&amp;C161&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Wilmer','JOHANSSON','20020009-6529');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Wilmer','JOHANSSON','20020018-3912');</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -6662,11 +6835,11 @@
       </c>
       <c r="F162" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19590023-8605</v>
+        <v>19590024-8494</v>
       </c>
       <c r="G162" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B162&amp;"','"&amp;C162&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jorge','JOFRE','19590023-8605');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jorge','JOFRE','19590024-8494');</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -6688,11 +6861,11 @@
       </c>
       <c r="F163" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19960005-6323</v>
+        <v>19960021-3741</v>
       </c>
       <c r="G163" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B163&amp;"','"&amp;C163&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Naemi','JAWOROWSKI','19960005-6323');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Naemi','JAWOROWSKI','19960021-3741');</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -6714,11 +6887,11 @@
       </c>
       <c r="F164" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020005-1991</v>
+        <v>20020012-8812</v>
       </c>
       <c r="G164" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B164&amp;"','"&amp;C164&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linnea','JARNROT','20020005-1991');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linnea','JARNROT','20020012-8812');</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -6740,11 +6913,11 @@
       </c>
       <c r="F165" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20000009-3998</v>
+        <v>20000008-9778</v>
       </c>
       <c r="G165" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B165&amp;"','"&amp;C165&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ludwig','JAHREN','20000009-3998');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ludwig','JAHREN','20000008-9778');</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -6766,11 +6939,11 @@
       </c>
       <c r="F166" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010029-8892</v>
+        <v>20010029-2424</v>
       </c>
       <c r="G166" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B166&amp;"','"&amp;C166&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linus','ISBRING','20010029-8892');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Linus','ISBRING','20010029-2424');</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -6792,11 +6965,11 @@
       </c>
       <c r="F167" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19860026-9674</v>
+        <v>19860003-4072</v>
       </c>
       <c r="G167" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B167&amp;"','"&amp;C167&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Thomas','IBURG','19860026-9674');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Thomas','IBURG','19860003-4072');</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -6818,11 +6991,11 @@
       </c>
       <c r="F168" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010003-7219</v>
+        <v>20010028-4049</v>
       </c>
       <c r="G168" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B168&amp;"','"&amp;C168&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Edvin ','HÖÖG','20010003-7219');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Edvin ','HÖÖG','20010028-4049');</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -6844,11 +7017,11 @@
       </c>
       <c r="F169" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020027-6288</v>
+        <v>20020003-7002</v>
       </c>
       <c r="G169" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B169&amp;"','"&amp;C169&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pontus','HÄLL','20020027-6288');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Pontus','HÄLL','20020003-7002');</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -6870,11 +7043,11 @@
       </c>
       <c r="F170" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20050018-5151</v>
+        <v>20050027-1769</v>
       </c>
       <c r="G170" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B170&amp;"','"&amp;C170&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Zigge','HYLÉN','20050018-5151');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Zigge','HYLÉN','20050027-1769');</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -6896,11 +7069,11 @@
       </c>
       <c r="F171" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020024-7750</v>
+        <v>20020018-9474</v>
       </c>
       <c r="G171" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B171&amp;"','"&amp;C171&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alex','HOLMSTRÖM','20020024-7750');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alex','HOLMSTRÖM','20020018-9474');</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -6922,11 +7095,11 @@
       </c>
       <c r="F172" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030024-2167</v>
+        <v>20030030-2095</v>
       </c>
       <c r="G172" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B172&amp;"','"&amp;C172&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonathan','HOLMSTRÖM','20030024-2167');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonathan','HOLMSTRÖM','20030030-2095');</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -6948,11 +7121,11 @@
       </c>
       <c r="F173" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19940023-7207</v>
+        <v>19940011-7422</v>
       </c>
       <c r="G173" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B173&amp;"','"&amp;C173&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karin','HOLMBERG','19940023-7207');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Karin','HOLMBERG','19940011-7422');</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -6974,11 +7147,11 @@
       </c>
       <c r="F174" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010021-5008</v>
+        <v>20010001-5602</v>
       </c>
       <c r="G174" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B174&amp;"','"&amp;C174&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','HOLM','20010021-5008');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Marcus','HOLM','20010001-5602');</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -7000,11 +7173,11 @@
       </c>
       <c r="F175" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19820007-8870</v>
+        <v>19820007-1064</v>
       </c>
       <c r="G175" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B175&amp;"','"&amp;C175&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonas','HJELT','19820007-8870');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jonas','HJELT','19820007-1064');</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -7026,11 +7199,11 @@
       </c>
       <c r="F176" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19970005-4754</v>
+        <v>19970003-2905</v>
       </c>
       <c r="G176" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B176&amp;"','"&amp;C176&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ebba','HERRLANDER','19970005-4754');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ebba','HERRLANDER','19970003-2905');</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -7052,11 +7225,11 @@
       </c>
       <c r="F177" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20020004-2114</v>
+        <v>20020026-5334</v>
       </c>
       <c r="G177" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B177&amp;"','"&amp;C177&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Olle','HERMODSSON','20020004-2114');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Olle','HERMODSSON','20020026-5334');</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -7078,11 +7251,11 @@
       </c>
       <c r="F178" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20000005-7628</v>
+        <v>20000018-7011</v>
       </c>
       <c r="G178" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B178&amp;"','"&amp;C178&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','HENRIKSSON','20000005-7628');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emil','HENRIKSSON','20000018-7011');</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -7104,11 +7277,11 @@
       </c>
       <c r="F179" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19980023-3325</v>
+        <v>19980009-7398</v>
       </c>
       <c r="G179" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B179&amp;"','"&amp;C179&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emma','HENRIKSSON','19980023-3325');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emma','HENRIKSSON','19980009-7398');</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -7130,11 +7303,11 @@
       </c>
       <c r="F180" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19980009-2078</v>
+        <v>19980013-3163</v>
       </c>
       <c r="G180" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B180&amp;"','"&amp;C180&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','HENNINGSSON','19980009-2078');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','HENNINGSSON','19980013-3163');</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -7156,11 +7329,11 @@
       </c>
       <c r="F181" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20000019-5309</v>
+        <v>20000019-1150</v>
       </c>
       <c r="G181" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B181&amp;"','"&amp;C181&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emma','HENNERFORS','20000019-5309');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Emma','HENNERFORS','20000019-1150');</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -7182,11 +7355,11 @@
       </c>
       <c r="F182" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19960022-3864</v>
+        <v>19960011-3491</v>
       </c>
       <c r="G182" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B182&amp;"','"&amp;C182&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Joar','HELLQVIST','19960022-3864');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Joar','HELLQVIST','19960011-3491');</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -7208,11 +7381,11 @@
       </c>
       <c r="F183" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030011-7134</v>
+        <v>20030004-2079</v>
       </c>
       <c r="G183" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B183&amp;"','"&amp;C183&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Malin','HELGESSON','20030011-7134');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Malin','HELGESSON','20030004-2079');</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -7234,11 +7407,11 @@
       </c>
       <c r="F184" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19910004-3939</v>
+        <v>19910024-4840</v>
       </c>
       <c r="G184" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B184&amp;"','"&amp;C184&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Malin','HEDSTRÖM','19910004-3939');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Malin','HEDSTRÖM','19910024-4840');</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -7260,11 +7433,11 @@
       </c>
       <c r="F185" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19960015-6134</v>
+        <v>19960013-4480</v>
       </c>
       <c r="G185" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B185&amp;"','"&amp;C185&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Milad','HASSAN','19960015-6134');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Milad','HASSAN','19960013-4480');</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -7286,11 +7459,11 @@
       </c>
       <c r="F186" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010019-1660</v>
+        <v>20010028-4346</v>
       </c>
       <c r="G186" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B186&amp;"','"&amp;C186&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alfred','HANSSON','20010019-1660');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alfred','HANSSON','20010028-4346');</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -7312,11 +7485,11 @@
       </c>
       <c r="F187" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030001-7011</v>
+        <v>20030002-4263</v>
       </c>
       <c r="G187" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B187&amp;"','"&amp;C187&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Frida','HAMMARSTEDT','20030001-7011');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Frida','HAMMARSTEDT','20030002-4263');</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -7338,11 +7511,11 @@
       </c>
       <c r="F188" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>19990016-1331</v>
+        <v>19990013-7031</v>
       </c>
       <c r="G188" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B188&amp;"','"&amp;C188&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jakob','HAJUM','19990016-1331');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jakob','HAJUM','19990013-7031');</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -7364,11 +7537,11 @@
       </c>
       <c r="F189" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010030-3465</v>
+        <v>20010012-9765</v>
       </c>
       <c r="G189" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B189&amp;"','"&amp;C189&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johannes','HAGMAN','20010030-3465');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johannes','HAGMAN','20010012-9765');</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -7390,11 +7563,11 @@
       </c>
       <c r="F190" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010030-8635</v>
+        <v>20010006-4149</v>
       </c>
       <c r="G190" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B190&amp;"','"&amp;C190&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Axel','GUSTAFSSON','20010030-8635');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Axel','GUSTAFSSON','20010006-4149');</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -7416,11 +7589,11 @@
       </c>
       <c r="F191" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20030026-3132</v>
+        <v>20030025-2876</v>
       </c>
       <c r="G191" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B191&amp;"','"&amp;C191&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Leo','GRUBER','20030026-3132');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Leo','GRUBER','20030025-2876');</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -7442,11 +7615,11 @@
       </c>
       <c r="F192" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010014-2038</v>
+        <v>20010025-8356</v>
       </c>
       <c r="G192" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B192&amp;"','"&amp;C192&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Matilda','GRIMSBO','20010014-2038');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Matilda','GRIMSBO','20010025-8356');</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -7468,11 +7641,11 @@
       </c>
       <c r="F193" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20010011-7097</v>
+        <v>20010027-3896</v>
       </c>
       <c r="G193" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B193&amp;"','"&amp;C193&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Douglas','GRANQUIST','20010011-7097');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Douglas','GRANQUIST','20010027-3896');</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -7494,11 +7667,11 @@
       </c>
       <c r="F194" t="str">
         <f t="shared" ref="F194:F256" ca="1" si="3">TEXT(RANDBETWEEN(DATE(D194,1,1),DATE(D194,12,31)),"ååååmmdd") &amp; "-" &amp; RANDBETWEEN(1000,9999)</f>
-        <v>20030007-7306</v>
+        <v>20030023-2413</v>
       </c>
       <c r="G194" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B194&amp;"','"&amp;C194&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tova','GRANBERG','20030007-7306');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Tova','GRANBERG','20030023-2413');</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -7520,11 +7693,11 @@
       </c>
       <c r="F195" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19940005-8822</v>
+        <v>19940002-3175</v>
       </c>
       <c r="G195" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B195&amp;"','"&amp;C195&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Erik','FRANSSON','19940005-8822');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Erik','FRANSSON','19940002-3175');</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -7546,11 +7719,11 @@
       </c>
       <c r="F196" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20010014-3487</v>
+        <v>20010003-3139</v>
       </c>
       <c r="G196" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B196&amp;"','"&amp;C196&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Birk','FORSBERG','20010014-3487');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Birk','FORSBERG','20010003-3139');</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -7572,11 +7745,11 @@
       </c>
       <c r="F197" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19900006-9831</v>
+        <v>19900005-9619</v>
       </c>
       <c r="G197" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B197&amp;"','"&amp;C197&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rasmus','FJELL','19900006-9831');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rasmus','FJELL','19900005-9619');</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -7598,11 +7771,11 @@
       </c>
       <c r="F198" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20030020-3386</v>
+        <v>20030013-8584</v>
       </c>
       <c r="G198" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B198&amp;"','"&amp;C198&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Saga','FALK','20030020-3386');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Saga','FALK','20030013-8584');</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -7624,11 +7797,11 @@
       </c>
       <c r="F199" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20010020-4602</v>
+        <v>20010022-4498</v>
       </c>
       <c r="G199" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B199&amp;"','"&amp;C199&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jennifer','ERNST','20010020-4602');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jennifer','ERNST','20010022-4498');</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -7650,11 +7823,11 @@
       </c>
       <c r="F200" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19980024-8883</v>
+        <v>19980006-6328</v>
       </c>
       <c r="G200" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B200&amp;"','"&amp;C200&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustaf','ENGSTRÖM','19980024-8883');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustaf','ENGSTRÖM','19980006-6328');</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -7676,11 +7849,11 @@
       </c>
       <c r="F201" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20040028-6603</v>
+        <v>20040001-1899</v>
       </c>
       <c r="G201" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B201&amp;"','"&amp;C201&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Andreas','ELIASSON','20040028-6603');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Andreas','ELIASSON','20040001-1899');</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -7702,11 +7875,11 @@
       </c>
       <c r="F202" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19970022-7725</v>
+        <v>19970008-5279</v>
       </c>
       <c r="G202" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B202&amp;"','"&amp;C202&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','ELIASSON','19970022-7725');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','ELIASSON','19970008-5279');</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -7728,11 +7901,11 @@
       </c>
       <c r="F203" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19930020-2816</v>
+        <v>19930028-7818</v>
       </c>
       <c r="G203" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B203&amp;"','"&amp;C203&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rebecca','ELIASSON','19930020-2816');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rebecca','ELIASSON','19930028-7818');</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -7754,11 +7927,11 @@
       </c>
       <c r="F204" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020017-6713</v>
+        <v>20020028-8843</v>
       </c>
       <c r="G204" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B204&amp;"','"&amp;C204&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Omar','EL-HAMS','20020017-6713');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Omar','EL-HAMS','20020028-8843');</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -7780,11 +7953,11 @@
       </c>
       <c r="F205" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20040030-7240</v>
+        <v>20040005-8609</v>
       </c>
       <c r="G205" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B205&amp;"','"&amp;C205&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','EKVALL','20040030-7240');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Elias','EKVALL','20040005-8609');</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -7806,11 +7979,11 @@
       </c>
       <c r="F206" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20050018-7648</v>
+        <v>20050018-1779</v>
       </c>
       <c r="G206" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B206&amp;"','"&amp;C206&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rasmus','EKVALL','20050018-7648');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Rasmus','EKVALL','20050018-1779');</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -7832,11 +8005,11 @@
       </c>
       <c r="F207" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020018-9819</v>
+        <v>20020026-3518</v>
       </c>
       <c r="G207" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B207&amp;"','"&amp;C207&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','EK .','20020018-9819');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','EK .','20020026-3518');</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -7858,11 +8031,11 @@
       </c>
       <c r="F208" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19980029-5510</v>
+        <v>19980002-3648</v>
       </c>
       <c r="G208" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B208&amp;"','"&amp;C208&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl','EDVINSSON','19980029-5510');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl','EDVINSSON','19980002-3648');</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -7884,11 +8057,11 @@
       </c>
       <c r="F209" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20000016-6329</v>
+        <v>20000011-8085</v>
       </c>
       <c r="G209" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B209&amp;"','"&amp;C209&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Markus','EDLUND','20000016-6329');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Markus','EDLUND','20000011-8085');</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -7910,11 +8083,11 @@
       </c>
       <c r="F210" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990022-1733</v>
+        <v>19990009-1506</v>
       </c>
       <c r="G210" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B210&amp;"','"&amp;C210&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sofie','EDHOLM','19990022-1733');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Sofie','EDHOLM','19990009-1506');</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -7936,11 +8109,11 @@
       </c>
       <c r="F211" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19950010-9515</v>
+        <v>19950019-9288</v>
       </c>
       <c r="G211" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B211&amp;"','"&amp;C211&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hasbulat','DUDUSHEV','19950010-9515');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hasbulat','DUDUSHEV','19950019-9288');</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -7962,11 +8135,11 @@
       </c>
       <c r="F212" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20000025-7283</v>
+        <v>20000011-9001</v>
       </c>
       <c r="G212" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B212&amp;"','"&amp;C212&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carolina','DJORDJEVSKI','20000025-7283');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carolina','DJORDJEVSKI','20000011-9001');</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -7988,11 +8161,11 @@
       </c>
       <c r="F213" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19970001-6560</v>
+        <v>19970023-8124</v>
       </c>
       <c r="G213" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B213&amp;"','"&amp;C213&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Armin','DIDIC','19970001-6560');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Armin','DIDIC','19970023-8124');</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -8014,11 +8187,11 @@
       </c>
       <c r="F214" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19890020-2615</v>
+        <v>19890031-4390</v>
       </c>
       <c r="G214" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B214&amp;"','"&amp;C214&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jeffrey','DENIAN','19890020-2615');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jeffrey','DENIAN','19890031-4390');</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -8040,11 +8213,11 @@
       </c>
       <c r="F215" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020029-5116</v>
+        <v>20020026-7043</v>
       </c>
       <c r="G215" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B215&amp;"','"&amp;C215&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Oskar','DANIELSSON','20020029-5116');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Oskar','DANIELSSON','20020026-7043');</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -8066,11 +8239,11 @@
       </c>
       <c r="F216" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020031-5441</v>
+        <v>20020016-6145</v>
       </c>
       <c r="G216" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B216&amp;"','"&amp;C216&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Zsolt','CSILLAG','20020031-5441');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Zsolt','CSILLAG','20020016-6145');</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
@@ -8092,11 +8265,11 @@
       </c>
       <c r="F217" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20040016-3522</v>
+        <v>20040024-6940</v>
       </c>
       <c r="G217" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B217&amp;"','"&amp;C217&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Teo','COSTA','20040016-3522');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Teo','COSTA','20040024-6940');</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -8118,11 +8291,11 @@
       </c>
       <c r="F218" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19880010-5331</v>
+        <v>19880022-1626</v>
       </c>
       <c r="G218" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B218&amp;"','"&amp;C218&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mathias','CLAUSSEN','19880010-5331');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Mathias','CLAUSSEN','19880022-1626');</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -8144,11 +8317,11 @@
       </c>
       <c r="F219" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990023-6474</v>
+        <v>19990028-6955</v>
       </c>
       <c r="G219" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B219&amp;"','"&amp;C219&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Adam','CHRISTIANSSON','19990023-6474');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Adam','CHRISTIANSSON','19990028-6955');</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -8170,11 +8343,11 @@
       </c>
       <c r="F220" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20040021-6315</v>
+        <v>20040020-5327</v>
       </c>
       <c r="G220" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B220&amp;"','"&amp;C220&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Max','CHRISTIANSSON','20040021-6315');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Max','CHRISTIANSSON','20040020-5327');</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -8196,11 +8369,11 @@
       </c>
       <c r="F221" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20000024-5693</v>
+        <v>20000028-6844</v>
       </c>
       <c r="G221" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B221&amp;"','"&amp;C221&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','CHRISTENSSON','20000024-5693');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexander','CHRISTENSSON','20000028-6844');</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -8222,11 +8395,11 @@
       </c>
       <c r="F222" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19950005-1512</v>
+        <v>19950013-3226</v>
       </c>
       <c r="G222" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B222&amp;"','"&amp;C222&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','BUSCH','19950005-1512');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Victor','BUSCH','19950013-3226');</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -8248,11 +8421,11 @@
       </c>
       <c r="F223" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990013-1494</v>
+        <v>19990028-8351</v>
       </c>
       <c r="G223" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B223&amp;"','"&amp;C223&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kajsa','BRYNFORS','19990013-1494');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Kajsa','BRYNFORS','19990028-8351');</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -8274,11 +8447,11 @@
       </c>
       <c r="F224" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20030016-1567</v>
+        <v>20030031-2294</v>
       </c>
       <c r="G224" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B224&amp;"','"&amp;C224&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jacob ','BORGSTRÖM','20030016-1567');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jacob ','BORGSTRÖM','20030031-2294');</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -8300,11 +8473,11 @@
       </c>
       <c r="F225" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19860027-7247</v>
+        <v>19860011-2786</v>
       </c>
       <c r="G225" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B225&amp;"','"&amp;C225&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('David','BORG-HANSEN','19860027-7247');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('David','BORG-HANSEN','19860011-2786');</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -8326,11 +8499,11 @@
       </c>
       <c r="F226" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20000018-1048</v>
+        <v>20000012-9706</v>
       </c>
       <c r="G226" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B226&amp;"','"&amp;C226&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jens','BOHN','20000018-1048');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jens','BOHN','20000012-9706');</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -8352,11 +8525,11 @@
       </c>
       <c r="F227" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990003-9538</v>
+        <v>19990024-6090</v>
       </c>
       <c r="G227" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B227&amp;"','"&amp;C227&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustav','BOHM','19990003-9538');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustav','BOHM','19990024-6090');</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -8378,11 +8551,11 @@
       </c>
       <c r="F228" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990011-2248</v>
+        <v>19990014-2632</v>
       </c>
       <c r="G228" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B228&amp;"','"&amp;C228&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ivar','BJÖRKQVIST','19990011-2248');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ivar','BJÖRKQVIST','19990014-2632');</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -8404,11 +8577,11 @@
       </c>
       <c r="F229" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20010027-4073</v>
+        <v>20010012-5145</v>
       </c>
       <c r="G229" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B229&amp;"','"&amp;C229&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl','BJÖRKLUND','20010027-4073');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Carl','BJÖRKLUND','20010012-5145');</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -8430,11 +8603,11 @@
       </c>
       <c r="F230" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20030028-3155</v>
+        <v>20030025-6382</v>
       </c>
       <c r="G230" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B230&amp;"','"&amp;C230&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Felix','BJÖRKLUND','20030028-3155');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Felix','BJÖRKLUND','20030025-6382');</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -8456,11 +8629,11 @@
       </c>
       <c r="F231" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19970004-3477</v>
+        <v>19970016-8726</v>
       </c>
       <c r="G231" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B231&amp;"','"&amp;C231&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','BJÖRKLUND','19970004-3477');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('William','BJÖRKLUND','19970016-8726');</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -8482,11 +8655,11 @@
       </c>
       <c r="F232" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20030028-5258</v>
+        <v>20030018-1067</v>
       </c>
       <c r="G232" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B232&amp;"','"&amp;C232&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Dante','BIONAZ GUSTAFSSON','20030028-5258');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Dante','BIONAZ GUSTAFSSON','20030018-1067');</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -8508,11 +8681,11 @@
       </c>
       <c r="F233" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020029-1192</v>
+        <v>20020003-3056</v>
       </c>
       <c r="G233" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B233&amp;"','"&amp;C233&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Joel','BERNTSSON','20020029-1192');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Joel','BERNTSSON','20020003-3056');</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -8534,11 +8707,11 @@
       </c>
       <c r="F234" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20000015-7185</v>
+        <v>20000024-3164</v>
       </c>
       <c r="G234" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B234&amp;"','"&amp;C234&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ola','BERGLUND','20000015-7185');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Ola','BERGLUND','20000024-3164');</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -8560,11 +8733,11 @@
       </c>
       <c r="F235" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020008-1612</v>
+        <v>20020014-5708</v>
       </c>
       <c r="G235" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B235&amp;"','"&amp;C235&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hannes','BERG','20020008-1612');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hannes','BERG','20020014-5708');</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -8586,11 +8759,11 @@
       </c>
       <c r="F236" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20040019-6518</v>
+        <v>20040019-7728</v>
       </c>
       <c r="G236" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B236&amp;"','"&amp;C236&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amir','BENTALIB','20040019-6518');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amir','BENTALIB','20040019-7728');</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -8612,11 +8785,11 @@
       </c>
       <c r="F237" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20030002-7783</v>
+        <v>20030031-9556</v>
       </c>
       <c r="G237" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B237&amp;"','"&amp;C237&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Felicia','BENGTSON','20030002-7783');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Felicia','BENGTSON','20030031-9556');</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -8638,11 +8811,11 @@
       </c>
       <c r="F238" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990030-8623</v>
+        <v>19990017-7607</v>
       </c>
       <c r="G238" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B238&amp;"','"&amp;C238&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Vincent','BANNURA','19990030-8623');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Vincent','BANNURA','19990017-7607');</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -8664,11 +8837,11 @@
       </c>
       <c r="F239" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19980023-1808</v>
+        <v>19980030-5963</v>
       </c>
       <c r="G239" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B239&amp;"','"&amp;C239&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hampus','ARVERUS','19980023-1808');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Hampus','ARVERUS','19980030-5963');</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
@@ -8690,11 +8863,11 @@
       </c>
       <c r="F240" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19900020-3129</v>
+        <v>19900019-2962</v>
       </c>
       <c r="G240" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B240&amp;"','"&amp;C240&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','ARONSSON','19900020-3129');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Johan','ARONSSON','19900019-2962');</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -8716,11 +8889,11 @@
       </c>
       <c r="F241" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020014-9965</v>
+        <v>20020026-1886</v>
       </c>
       <c r="G241" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B241&amp;"','"&amp;C241&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alba','ARGUETA','20020014-9965');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alba','ARGUETA','20020026-1886');</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -8742,11 +8915,11 @@
       </c>
       <c r="F242" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20010014-8596</v>
+        <v>20010018-3531</v>
       </c>
       <c r="G242" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B242&amp;"','"&amp;C242&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexandro','ARGUETA','20010014-8596');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Alexandro','ARGUETA','20010018-3531');</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -8768,11 +8941,11 @@
       </c>
       <c r="F243" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20020006-5503</v>
+        <v>20020014-4937</v>
       </c>
       <c r="G243" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B243&amp;"','"&amp;C243&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Laura','ANTVORSKOV','20020006-5503');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Laura','ANTVORSKOV','20020014-4937');</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -8794,11 +8967,11 @@
       </c>
       <c r="F244" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19840003-1478</v>
+        <v>19840001-7637</v>
       </c>
       <c r="G244" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B244&amp;"','"&amp;C244&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jennie','ANDRÉASON','19840003-1478');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jennie','ANDRÉASON','19840001-7637');</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -8820,11 +8993,11 @@
       </c>
       <c r="F245" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20000022-7843</v>
+        <v>20000020-7348</v>
       </c>
       <c r="G245" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B245&amp;"','"&amp;C245&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amanda','ANDERSSON','20000022-7843');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amanda','ANDERSSON','20000020-7348');</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -8846,11 +9019,11 @@
       </c>
       <c r="F246" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19980003-7897</v>
+        <v>19980027-8520</v>
       </c>
       <c r="G246" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B246&amp;"','"&amp;C246&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Daniel','ANDERSSON','19980003-7897');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Daniel','ANDERSSON','19980027-8520');</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -8872,11 +9045,11 @@
       </c>
       <c r="F247" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990022-7660</v>
+        <v>19990022-2945</v>
       </c>
       <c r="G247" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B247&amp;"','"&amp;C247&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Isak','ANDERSSON','19990022-7660');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Isak','ANDERSSON','19990022-2945');</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -8898,11 +9071,11 @@
       </c>
       <c r="F248" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20050015-7689</v>
+        <v>20050021-1141</v>
       </c>
       <c r="G248" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B248&amp;"','"&amp;C248&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Lisa','ANDERSSON','20050015-7689');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Lisa','ANDERSSON','20050021-1141');</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -8924,11 +9097,11 @@
       </c>
       <c r="F249" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20030026-6378</v>
+        <v>20030011-4082</v>
       </c>
       <c r="G249" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B249&amp;"','"&amp;C249&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Max','ANDERSSON','20030026-6378');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Max','ANDERSSON','20030011-4082');</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -8950,11 +9123,11 @@
       </c>
       <c r="F250" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20040017-2341</v>
+        <v>20040025-2296</v>
       </c>
       <c r="G250" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B250&amp;"','"&amp;C250&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Razmus','ANDERSSON','20040017-2341');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Razmus','ANDERSSON','20040025-2296');</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -8976,11 +9149,11 @@
       </c>
       <c r="F251" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20000028-1907</v>
+        <v>20000003-5243</v>
       </c>
       <c r="G251" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B251&amp;"','"&amp;C251&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Simon','ANDERSSON','20000028-1907');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Simon','ANDERSSON','20000003-5243');</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -9002,11 +9175,11 @@
       </c>
       <c r="F252" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19950006-3724</v>
+        <v>19950020-1895</v>
       </c>
       <c r="G252" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B252&amp;"','"&amp;C252&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Siber','AHMED','19950006-3724');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Siber','AHMED','19950020-1895');</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -9028,11 +9201,11 @@
       </c>
       <c r="F253" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19920018-3522</v>
+        <v>19920001-7479</v>
       </c>
       <c r="G253" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B253&amp;"','"&amp;C253&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Frederik','AGERTOFT','19920018-3522');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Frederik','AGERTOFT','19920001-7479');</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -9054,11 +9227,11 @@
       </c>
       <c r="F254" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19990015-2792</v>
+        <v>19990015-4055</v>
       </c>
       <c r="G254" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B254&amp;"','"&amp;C254&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jacob','AGERTOFT','19990015-2792');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Jacob','AGERTOFT','19990015-4055');</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -9080,11 +9253,11 @@
       </c>
       <c r="F255" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20010005-7410</v>
+        <v>20010003-3205</v>
       </c>
       <c r="G255" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B255&amp;"','"&amp;C255&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amgad','ABU-RAMADAN','20010005-7410');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Amgad','ABU-RAMADAN','20010003-3205');</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -9106,11 +9279,11 @@
       </c>
       <c r="F256" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19970029-7852</v>
+        <v>19970008-1901</v>
       </c>
       <c r="G256" t="str">
         <f ca="1">"INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('"&amp;B256&amp;"','"&amp;C256&amp;"','"&amp;Tabell5[[#This Row],[Personnumber]]&amp;"');"</f>
-        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustaf','A-BROLIN','19970029-7852');</v>
+        <v>INSERT INTO Judokas (FirstName, LastName, Personnumber) VALUES ('Gustaf','A-BROLIN','19970008-1901');</v>
       </c>
     </row>
   </sheetData>
@@ -9119,4 +9292,478 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="113.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42687</v>
+      </c>
+      <c r="C2" t="s">
+        <v>498</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"insert into Competitions (Name, Location, EventDate) VALUES('"&amp;C2&amp;"', '"&amp;A2&amp;"','"&amp;TEXT(B2,"åååå-MM-dd")&amp;"');"</f>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Skåneserien IV', ' Staffanstorp','2016-11-13');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42686</v>
+      </c>
+      <c r="C3" t="s">
+        <v>499</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D30" si="0">"insert into Competitions (Name, Location, EventDate) VALUES('"&amp;C3&amp;"', '"&amp;A3&amp;"','"&amp;TEXT(B3,"åååå-MM-dd")&amp;"');"</f>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('SydCup IV och Veteran SM', ' Staffanstorp','2016-11-12');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B4" s="3">
+        <v>42679</v>
+      </c>
+      <c r="C4" t="s">
+        <v>500</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('-06 Adidas Challenge', ' Borås','2016-11-05');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>483</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42665</v>
+      </c>
+      <c r="C5" t="s">
+        <v>501</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('National-Cup', ' Halmstad','2016-10-22');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>484</v>
+      </c>
+      <c r="B6" s="3">
+        <v>42665</v>
+      </c>
+      <c r="C6" t="s">
+        <v>502</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('GoCup II', ' Stenungsund','2016-10-22');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B7" s="3">
+        <v>42658</v>
+      </c>
+      <c r="C7" t="s">
+        <v>503</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Södra Judo Open III', ' Haninge','2016-10-15');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>485</v>
+      </c>
+      <c r="B8" s="3">
+        <v>42652</v>
+      </c>
+      <c r="C8" t="s">
+        <v>504</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Skåneserien 3', ' Skurup','2016-10-09');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B9" s="3">
+        <v>42651</v>
+      </c>
+      <c r="C9" t="s">
+        <v>505</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('SydCup 3', ' Skurup','2016-10-08');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>486</v>
+      </c>
+      <c r="B10" s="3">
+        <v>42651</v>
+      </c>
+      <c r="C10" t="s">
+        <v>506</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Norra Norrlands DM', ' Vilhelmina','2016-10-08');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>487</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42644</v>
+      </c>
+      <c r="C11" t="s">
+        <v>507</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Linde Judo Open', ' Lindesberg','2016-10-01');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>488</v>
+      </c>
+      <c r="B12" s="3">
+        <v>42637</v>
+      </c>
+      <c r="C12" t="s">
+        <v>508</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Junior Swedish Open (J-Swop)', ' Stockholm','2016-09-24');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>480</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42630</v>
+      </c>
+      <c r="C13" t="s">
+        <v>509</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Borlänge Judo Open Resultat', 'Borlänge','2016-09-17');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>489</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42623</v>
+      </c>
+      <c r="C14" t="s">
+        <v>510</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Gothenburg Judo Open', ' Göteborg','2016-09-10');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>490</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42504</v>
+      </c>
+      <c r="C15" t="s">
+        <v>511</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Sundsvallscup', ' Sundsvall','2016-05-14');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>491</v>
+      </c>
+      <c r="B16" s="3">
+        <v>42495</v>
+      </c>
+      <c r="C16" t="s">
+        <v>512</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Budo-Nord Cup', ' Lund','2016-05-05');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>492</v>
+      </c>
+      <c r="B17" s="3">
+        <v>42484</v>
+      </c>
+      <c r="C17" t="s">
+        <v>513</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Skåne-Serien II', ' Genarp','2016-04-24');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>497</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42483</v>
+      </c>
+      <c r="C18" t="s">
+        <v>514</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('-24 Trollträffen I', ' Älvhögsborg','2016-04-23');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>479</v>
+      </c>
+      <c r="B19" s="3">
+        <v>42476</v>
+      </c>
+      <c r="C19" t="s">
+        <v>515</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Senior SM 2016', ' Haninge','2016-04-16');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>479</v>
+      </c>
+      <c r="B20" s="3">
+        <v>42476</v>
+      </c>
+      <c r="C20" t="s">
+        <v>516</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Södra Judo Open 2', ' Haninge','2016-04-16');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>493</v>
+      </c>
+      <c r="B21" s="3">
+        <v>42462</v>
+      </c>
+      <c r="C21" t="s">
+        <v>517</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Sörmlandsträffen', ' Oxelösund','2016-04-02');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>484</v>
+      </c>
+      <c r="B22" s="3">
+        <v>42448</v>
+      </c>
+      <c r="C22" t="s">
+        <v>518</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Go Cup', ' Stenungsund','2016-03-19');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>494</v>
+      </c>
+      <c r="B23" s="3">
+        <v>42441</v>
+      </c>
+      <c r="C23" t="s">
+        <v>519</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Sun City Judo Open', ' Karlstad','2016-03-12');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>490</v>
+      </c>
+      <c r="B24" s="3">
+        <v>42427</v>
+      </c>
+      <c r="C24" t="s">
+        <v>520</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Drakstadens Judo Cup', ' Sundsvall','2016-02-27');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>482</v>
+      </c>
+      <c r="B25" s="3">
+        <v>42414</v>
+      </c>
+      <c r="C25" t="s">
+        <v>521</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Adidas Challenge', ' Borås','2016-02-14');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>482</v>
+      </c>
+      <c r="B26" s="3">
+        <v>42413</v>
+      </c>
+      <c r="C26" t="s">
+        <v>522</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Junior och Kadett SM', ' Borås','2016-02-13');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>495</v>
+      </c>
+      <c r="B27" s="3">
+        <v>42406</v>
+      </c>
+      <c r="C27" t="s">
+        <v>523</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Helsingborg Judo Open', ' Helsingborg','2016-02-06');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>479</v>
+      </c>
+      <c r="B28" s="3">
+        <v>42406</v>
+      </c>
+      <c r="C28" t="s">
+        <v>524</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Södra Judo Open I', ' Haninge','2016-02-06');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>496</v>
+      </c>
+      <c r="B29" s="3">
+        <v>42379</v>
+      </c>
+      <c r="C29" t="s">
+        <v>525</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Skåneserien I', ' Kristianstad','2016-01-10');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>496</v>
+      </c>
+      <c r="B30" s="3">
+        <v>42378</v>
+      </c>
+      <c r="C30" t="s">
+        <v>526</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Competitions (Name, Location, EventDate) VALUES('Kristianstad Judo Open Resultat', ' Kristianstad','2016-01-09');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>